<commit_message>
rename class and add new
</commit_message>
<xml_diff>
--- a/src/main/resources/data/data.xlsx
+++ b/src/main/resources/data/data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\diplom\face-detection2\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F32E34-FDC1-4881-BFD0-9DB146AF6969}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234852B7-69D9-4AF1-A6F1-DB4D07142757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3255" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{F58CB082-2D72-4BBF-A651-2245285DBC37}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,11 +31,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+  <si>
+    <t>Андрей</t>
+  </si>
+  <si>
+    <t>Степченков</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>Рабочий</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2023-06-05</t>
+  </si>
+  <si>
+    <t>16:58</t>
+  </si>
+  <si>
+    <t>16:59</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,14 +408,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703F8718-4D34-42E8-B196-0AF043864ACB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:H3"/>
+      <selection activeCell="J8" sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>